<commit_message>
CloudFare, Hono --> Started
</commit_message>
<xml_diff>
--- a/TOPICS_COHORT.xlsx
+++ b/TOPICS_COHORT.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27531"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MERN\myRepo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64F16196-A42D-4292-839F-B3FCCFFF101F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05E970FE-4289-4AF3-97F1-FF2F5EE06267}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30255" yWindow="1440" windowWidth="17250" windowHeight="8865" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TOPICS" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="63">
   <si>
     <t>SUB TOPICS</t>
   </si>
@@ -208,6 +208,12 @@
   </si>
   <si>
     <t>Autogenerated Client (Prisma)</t>
+  </si>
+  <si>
+    <t>Serverless Fns</t>
+  </si>
+  <si>
+    <t>Hono</t>
   </si>
 </sst>
 </file>
@@ -686,10 +692,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:A34"/>
+  <dimension ref="A1:A38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A34" sqref="A34"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="H37" sqref="H37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -815,6 +821,16 @@
     <row r="34" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A34" s="14" t="s">
         <v>60</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A36" s="14" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A38" s="14" t="s">
+        <v>62</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Topics --> AWS Cloudfront --> S3 --> Deployment
</commit_message>
<xml_diff>
--- a/TOPICS_COHORT.xlsx
+++ b/TOPICS_COHORT.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MERN\myRepo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA46C902-8FEE-459A-86BB-A9A8C23953AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{490DD9DA-7B33-4599-A1B7-194C0863CBE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="74">
   <si>
     <t>SUB TOPICS</t>
   </si>
@@ -265,6 +265,12 @@
   </si>
   <si>
     <t>https://certbot.eff.org/  --&gt; A free alternative to generate certificates for you websites</t>
+  </si>
+  <si>
+    <t>CDN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Deploying Frontends on AWS --&gt;  Cloudfront --&gt; S3 </t>
   </si>
 </sst>
 </file>
@@ -757,10 +763,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:A46"/>
+  <dimension ref="A1:A50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="Q36" sqref="Q36"/>
+    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
+      <selection activeCell="Q46" sqref="Q46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -916,6 +922,16 @@
     <row r="46" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A46" s="15" t="s">
         <v>70</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A48" s="15" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A50" s="15" t="s">
+        <v>72</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated Topics --> Monorepos & NPM Deploy
</commit_message>
<xml_diff>
--- a/TOPICS_COHORT.xlsx
+++ b/TOPICS_COHORT.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MERN\myRepo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{490DD9DA-7B33-4599-A1B7-194C0863CBE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33BE1794-2D17-49F7-BFAF-7E1036F796FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="76">
   <si>
     <t>SUB TOPICS</t>
   </si>
@@ -271,6 +271,12 @@
   </si>
   <si>
     <t xml:space="preserve">Deploying Frontends on AWS --&gt;  Cloudfront --&gt; S3 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Deploying NPM </t>
+  </si>
+  <si>
+    <t>Monoreps --&gt; TurboRepo</t>
   </si>
 </sst>
 </file>
@@ -763,10 +769,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:A50"/>
+  <dimension ref="A1:A54"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
-      <selection activeCell="Q46" sqref="Q46"/>
+      <selection activeCell="M47" sqref="M47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -932,6 +938,16 @@
     <row r="50" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A50" s="15" t="s">
         <v>72</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A52" s="15" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A54" s="15" t="s">
+        <v>75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Started Docker and Updated TOPICS
</commit_message>
<xml_diff>
--- a/TOPICS_COHORT.xlsx
+++ b/TOPICS_COHORT.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MERN\myRepo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33BE1794-2D17-49F7-BFAF-7E1036F796FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3146E0F-56C8-4483-BD02-894FBAF1D9C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="77">
   <si>
     <t>SUB TOPICS</t>
   </si>
@@ -277,6 +277,9 @@
   </si>
   <si>
     <t>Monoreps --&gt; TurboRepo</t>
+  </si>
+  <si>
+    <t>Actionable Docker</t>
   </si>
 </sst>
 </file>
@@ -769,10 +772,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:A54"/>
+  <dimension ref="A1:A56"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
-      <selection activeCell="M47" sqref="M47"/>
+      <selection activeCell="R53" sqref="R53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -948,6 +951,11 @@
     <row r="54" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A54" s="15" t="s">
         <v>75</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A56" s="15" t="s">
+        <v>76</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Prisma Connection Pool Updated
</commit_message>
<xml_diff>
--- a/TOPICS_COHORT.xlsx
+++ b/TOPICS_COHORT.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="79">
   <si>
     <t>SUB TOPICS</t>
   </si>
@@ -282,6 +282,9 @@
   </si>
   <si>
     <t>Connection Pooling</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Prima Accelerate For Connection Pooling </t>
   </si>
 </sst>
 </file>
@@ -774,10 +777,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:A58"/>
+  <dimension ref="A1:A60"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="J49" sqref="J49"/>
+      <selection activeCell="J54" sqref="J54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -963,6 +966,11 @@
     <row r="58" spans="1:1">
       <c r="A58" s="15" t="s">
         <v>77</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" ht="28.8">
+      <c r="A60" s="15" t="s">
+        <v>78</v>
       </c>
     </row>
   </sheetData>
@@ -1096,7 +1104,7 @@
     <row r="7" spans="1:1">
       <c r="A7" s="1"/>
     </row>
-    <row r="8" spans="1:1" ht="28.8">
+    <row r="8" spans="1:1">
       <c r="A8" s="9" t="s">
         <v>30</v>
       </c>

</xml_diff>